<commit_message>
add few items in instrument data-file for parsing
</commit_message>
<xml_diff>
--- a/data/Instrument_prices.xlsx
+++ b/data/Instrument_prices.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3065" uniqueCount="3026">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3296" uniqueCount="3115">
   <si>
     <t xml:space="preserve">наш код</t>
   </si>
@@ -9098,6 +9098,273 @@
   </si>
   <si>
     <t xml:space="preserve">000046287</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000081400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Аккумулятор 3 шт + ЗУ ASC30 Metabo Basic-Set 5.2  Li</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://instrument.ms/raskhodnye-materialy-i-osnastka/osnastka-dlya-elektroinstrumenta/akkumulyatory-dlya-instrumenta/tm-metabo/akkumulator-3-st-zu-asc30-metabo-basic-set-52-lihd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000086113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000083325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000086118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000083324</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000099035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Аккумуляторный шуруповерт Metabo BS 14,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-metabo/akkumulatornyj-surupovert-metabo-bs-144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000088932</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000059797</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000074712</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000091496</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000091835</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000091836</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000082961</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000061489</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000084285</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000085458</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000085466</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000044144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Аккумуляторный шуруповерт Metabo PowerMaxx BS-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000057550</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000063130</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000074920</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Лента пильная Metabo BAS-260 1712х6х0,36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://instrument.ms/raskhodnye-materialy-i-osnastka/osnastka-dlya-stankov/pilnye-polotna/tm-metabo/lenta-pilnaa-metabo-bas-260-1712h6h036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000078327</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Лобзик Metabo STEB 140 Plus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://instrument.ms/elektroinstrument/lobziki-i-sabelnye-pily/lobziki/tm-metabo/lobzik-metabo-steb-140-plus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000057549</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000044087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000071366</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000099031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Машина шлифовальная прямая Metabo DG 25 Set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://instrument.ms/pnevmaticheskoe-oborudovanie/pnevmoinstrument/pnevmoshlifovalnye-mashiny-pryamye/tm-metabo/masina-slifovalnaa-pramaa-metabo-dg-25-set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000073593</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ножи к рейсмусу МЕТАВО DH330 Metabo HSS 332</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://instrument.ms/raskhodnye-materialy-i-osnastka/osnastka-dlya-stankov/nozhi-k-stankam/tm-metabo/nozhi-k-reismusu-metavo-dh330-metabo-hss-332</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Отрезной круг по металлу Metabo 125х2,5х22 SP-Novoflex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000086107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Отрезной круг по металлу+ нержавейке Metabo 125х1,0х22 SP-Novorapid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://instrument.ms/raskhodnye-materialy-i-osnastka/osnastka-dlya-elektroinstrumenta/krugi-otreznye/tm-metabo/otreznoj-krug-po-metallu-nerzavejke-metabo-125h10h22-sp-novorapid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000098624</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Перфоратор SDS max Metabo KHEV 5-40 BL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://instrument.ms/elektroinstrument/perforatory/perforatory-sds-max/tm-metabo/perforator-sds-max-metabo-knev-5-40-bl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000073825</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000082962</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000070179</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000067530</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000070181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000086103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000046292</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000097970</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Пила дисковая Metabo KS 66 FS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://instrument.ms/elektroinstrument/pily-diskovye/pily-diskovye-setevye/tm-metabo/pila-diskovaa-metabo-ks-66-fs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000078336</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000044096</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000044097</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000070106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000044098</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000075080</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000046291</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000077185</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сумка для инструмента Metabo Малая</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://instrument.ms/raskhodnye-materialy-i-osnastka/osnastka-dlya-elektroinstrumenta/komplektuyushchie-i-zapchasti-dlya-elektroinstrumenta/tm-metabo/sumka-dla-instrumenta-metabo-malaa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000085468</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000085437</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000085464</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000093025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000059125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000087955</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Шлифмашина угловая Metabo WE 2000-230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/slifmasina-uglovaa-metabo-we-2000-230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000086720</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Шлифмашина угловая Metabo WE 2200-230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/slifmasina-uglovaa-metabo-we-2200-230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000051961</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Шлифмашина угловая Metabo WE 24-230 MVT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/slifmasina-uglovaa-metabo-we-24-230-mvt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000092780</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000095359</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Шлифмашина угловая Metabo WQ 1100-125 Quick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/slifmasina-uglovaa-metabo-wq-1100-125-quick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000072883</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000099034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Шлифмашина эксцентриковая Metabo SXE 3125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://instrument.ms/elektroinstrument/shlifovalnye-mashiny/shlifmashiny-ekstsentrikovye/tm-metabo/slifmasina-ekscentrikovaa-metabo-sxe-3125</t>
   </si>
 </sst>
 </file>
@@ -9109,7 +9376,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -9183,6 +9450,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -9244,7 +9518,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -9311,6 +9585,14 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -9415,14 +9697,14 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A397" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A521" activeCellId="0" sqref="A521"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1046" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1158" activeCellId="0" sqref="C1158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="77.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="77.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="12.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="7" style="0" width="8.63"/>
@@ -28508,83 +28790,853 @@
       <c r="Z1077" s="2"/>
       <c r="AA1077" s="2"/>
     </row>
-    <row r="1078" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1079" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1080" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1081" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1082" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1083" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1084" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1085" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1086" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1087" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1088" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1089" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1090" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1091" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1092" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1093" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1094" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1095" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1096" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1097" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1098" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1099" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1078" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1078" s="17" t="s">
+        <v>3026</v>
+      </c>
+      <c r="B1078" s="17" t="s">
+        <v>3027</v>
+      </c>
+      <c r="C1078" s="18" t="s">
+        <v>3028</v>
+      </c>
+    </row>
+    <row r="1079" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1079" s="17" t="s">
+        <v>2970</v>
+      </c>
+      <c r="B1079" s="17" t="s">
+        <v>2971</v>
+      </c>
+      <c r="C1079" s="18" t="s">
+        <v>2972</v>
+      </c>
+    </row>
+    <row r="1080" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1080" s="17" t="s">
+        <v>2973</v>
+      </c>
+      <c r="B1080" s="17" t="s">
+        <v>2974</v>
+      </c>
+      <c r="C1080" s="18" t="s">
+        <v>2975</v>
+      </c>
+    </row>
+    <row r="1081" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1081" s="17" t="s">
+        <v>3029</v>
+      </c>
+      <c r="B1081" s="17" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C1081" s="18" t="s">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="1082" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1082" s="17" t="s">
+        <v>3030</v>
+      </c>
+      <c r="B1082" s="17" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C1082" s="18" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="1083" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1083" s="17" t="s">
+        <v>3031</v>
+      </c>
+      <c r="B1083" s="17" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C1083" s="18" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="1084" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1084" s="17" t="s">
+        <v>3032</v>
+      </c>
+      <c r="B1084" s="17" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C1084" s="18" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="1085" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1085" s="17" t="s">
+        <v>3033</v>
+      </c>
+      <c r="B1085" s="17" t="s">
+        <v>3034</v>
+      </c>
+      <c r="C1085" s="18" t="s">
+        <v>3035</v>
+      </c>
+    </row>
+    <row r="1086" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1086" s="17" t="s">
+        <v>3036</v>
+      </c>
+      <c r="B1086" s="17" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C1086" s="18" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="1087" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1087" s="17" t="s">
+        <v>3037</v>
+      </c>
+      <c r="B1087" s="17" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C1087" s="18" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="1088" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1088" s="17" t="s">
+        <v>3038</v>
+      </c>
+      <c r="B1088" s="17" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C1088" s="18" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="1089" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1089" s="17" t="s">
+        <v>3039</v>
+      </c>
+      <c r="B1089" s="17" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C1089" s="18" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="1090" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1090" s="17" t="s">
+        <v>3040</v>
+      </c>
+      <c r="B1090" s="17" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C1090" s="18" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="1091" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1091" s="17" t="s">
+        <v>3041</v>
+      </c>
+      <c r="B1091" s="17" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C1091" s="18" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="1092" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1092" s="17" t="s">
+        <v>2979</v>
+      </c>
+      <c r="B1092" s="17" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C1092" s="18" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="1093" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1093" s="17" t="s">
+        <v>3042</v>
+      </c>
+      <c r="B1093" s="17" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C1093" s="18" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="1094" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1094" s="17" t="s">
+        <v>3043</v>
+      </c>
+      <c r="B1094" s="17" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C1094" s="18" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="1095" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1095" s="17" t="s">
+        <v>3044</v>
+      </c>
+      <c r="B1095" s="17" t="s">
+        <v>1293</v>
+      </c>
+      <c r="C1095" s="18" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="1096" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1096" s="17" t="s">
+        <v>2980</v>
+      </c>
+      <c r="B1096" s="17" t="s">
+        <v>1293</v>
+      </c>
+      <c r="C1096" s="18" t="s">
+        <v>2981</v>
+      </c>
+    </row>
+    <row r="1097" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1097" s="17" t="s">
+        <v>3045</v>
+      </c>
+      <c r="B1097" s="17" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C1097" s="18" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="1098" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1098" s="17" t="s">
+        <v>3046</v>
+      </c>
+      <c r="B1098" s="17" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C1098" s="18" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="1099" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1099" s="17" t="s">
+        <v>3047</v>
+      </c>
+      <c r="B1099" s="17" t="s">
+        <v>3048</v>
+      </c>
+      <c r="C1099" s="18" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="1100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1100" s="17" t="s">
+        <v>3049</v>
+      </c>
+      <c r="B1100" s="17" t="s">
+        <v>1308</v>
+      </c>
+      <c r="C1100" s="18" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="1101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1101" s="17" t="s">
+        <v>3050</v>
+      </c>
+      <c r="B1101" s="17" t="s">
+        <v>1308</v>
+      </c>
+      <c r="C1101" s="18" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="1102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1102" s="17" t="s">
+        <v>2982</v>
+      </c>
+      <c r="B1102" s="17" t="s">
+        <v>2983</v>
+      </c>
+      <c r="C1102" s="18" t="s">
+        <v>2984</v>
+      </c>
+    </row>
+    <row r="1103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1103" s="17" t="s">
+        <v>3051</v>
+      </c>
+      <c r="B1103" s="17" t="s">
+        <v>3052</v>
+      </c>
+      <c r="C1103" s="18" t="s">
+        <v>3053</v>
+      </c>
+    </row>
+    <row r="1104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1104" s="17" t="s">
+        <v>3054</v>
+      </c>
+      <c r="B1104" s="17" t="s">
+        <v>3055</v>
+      </c>
+      <c r="C1104" s="18" t="s">
+        <v>3056</v>
+      </c>
+    </row>
+    <row r="1105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1105" s="17" t="s">
+        <v>3057</v>
+      </c>
+      <c r="B1105" s="17" t="s">
+        <v>1318</v>
+      </c>
+      <c r="C1105" s="18" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="1106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1106" s="17" t="s">
+        <v>3058</v>
+      </c>
+      <c r="B1106" s="17" t="s">
+        <v>1320</v>
+      </c>
+      <c r="C1106" s="18" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="1107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1107" s="17" t="s">
+        <v>3059</v>
+      </c>
+      <c r="B1107" s="17" t="s">
+        <v>1322</v>
+      </c>
+      <c r="C1107" s="18" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="1108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1108" s="17" t="s">
+        <v>3060</v>
+      </c>
+      <c r="B1108" s="17" t="s">
+        <v>3061</v>
+      </c>
+      <c r="C1108" s="18" t="s">
+        <v>3062</v>
+      </c>
+    </row>
+    <row r="1109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1109" s="17" t="s">
+        <v>2985</v>
+      </c>
+      <c r="B1109" s="17" t="s">
+        <v>2986</v>
+      </c>
+      <c r="C1109" s="18" t="s">
+        <v>2987</v>
+      </c>
+    </row>
+    <row r="1110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1110" s="17" t="s">
+        <v>2988</v>
+      </c>
+      <c r="B1110" s="17" t="s">
+        <v>2989</v>
+      </c>
+      <c r="C1110" s="18" t="s">
+        <v>2990</v>
+      </c>
+    </row>
+    <row r="1111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1111" s="17" t="s">
+        <v>2991</v>
+      </c>
+      <c r="B1111" s="17" t="s">
+        <v>2992</v>
+      </c>
+      <c r="C1111" s="18" t="s">
+        <v>2993</v>
+      </c>
+    </row>
+    <row r="1112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1112" s="17" t="s">
+        <v>2994</v>
+      </c>
+      <c r="B1112" s="17" t="s">
+        <v>2995</v>
+      </c>
+      <c r="C1112" s="18" t="s">
+        <v>2996</v>
+      </c>
+    </row>
+    <row r="1113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1113" s="17" t="s">
+        <v>2997</v>
+      </c>
+      <c r="B1113" s="17" t="s">
+        <v>2998</v>
+      </c>
+      <c r="C1113" s="18" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1114" s="17" t="s">
+        <v>3000</v>
+      </c>
+      <c r="B1114" s="17" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C1114" s="18" t="s">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="1115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1115" s="17" t="s">
+        <v>3003</v>
+      </c>
+      <c r="B1115" s="17" t="s">
+        <v>1334</v>
+      </c>
+      <c r="C1115" s="18" t="s">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="1116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1116" s="17" t="s">
+        <v>3063</v>
+      </c>
+      <c r="B1116" s="17" t="s">
+        <v>3064</v>
+      </c>
+      <c r="C1116" s="18" t="s">
+        <v>3065</v>
+      </c>
+    </row>
+    <row r="1117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1117" s="17" t="s">
+        <v>3004</v>
+      </c>
+      <c r="B1117" s="17" t="s">
+        <v>3066</v>
+      </c>
+      <c r="C1117" s="18" t="s">
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="1118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1118" s="17" t="s">
+        <v>3067</v>
+      </c>
+      <c r="B1118" s="17" t="s">
+        <v>3068</v>
+      </c>
+      <c r="C1118" s="18" t="s">
+        <v>3069</v>
+      </c>
+    </row>
+    <row r="1119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1119" s="17" t="s">
+        <v>3007</v>
+      </c>
+      <c r="B1119" s="17" t="s">
+        <v>3008</v>
+      </c>
+      <c r="C1119" s="18" t="s">
+        <v>3009</v>
+      </c>
+    </row>
+    <row r="1120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1120" s="17" t="s">
+        <v>3010</v>
+      </c>
+      <c r="B1120" s="17" t="s">
+        <v>3011</v>
+      </c>
+      <c r="C1120" s="18" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="1121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1121" s="17" t="s">
+        <v>3070</v>
+      </c>
+      <c r="B1121" s="17" t="s">
+        <v>3071</v>
+      </c>
+      <c r="C1121" s="18" t="s">
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="1122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1122" s="17" t="s">
+        <v>3073</v>
+      </c>
+      <c r="B1122" s="17" t="s">
+        <v>1336</v>
+      </c>
+      <c r="C1122" s="18" t="s">
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="1123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1123" s="17" t="s">
+        <v>3074</v>
+      </c>
+      <c r="B1123" s="17" t="s">
+        <v>1338</v>
+      </c>
+      <c r="C1123" s="18" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="1124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1124" s="17" t="s">
+        <v>3075</v>
+      </c>
+      <c r="B1124" s="17" t="s">
+        <v>1340</v>
+      </c>
+      <c r="C1124" s="18" t="s">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="1125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1125" s="17" t="s">
+        <v>3076</v>
+      </c>
+      <c r="B1125" s="17" t="s">
+        <v>1342</v>
+      </c>
+      <c r="C1125" s="18" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="1126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1126" s="17" t="s">
+        <v>3077</v>
+      </c>
+      <c r="B1126" s="17" t="s">
+        <v>1344</v>
+      </c>
+      <c r="C1126" s="18" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="1127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1127" s="17" t="s">
+        <v>3078</v>
+      </c>
+      <c r="B1127" s="17" t="s">
+        <v>1346</v>
+      </c>
+      <c r="C1127" s="18" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="1128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1128" s="17" t="s">
+        <v>3079</v>
+      </c>
+      <c r="B1128" s="17" t="s">
+        <v>1352</v>
+      </c>
+      <c r="C1128" s="18" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="1129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1129" s="17" t="s">
+        <v>3080</v>
+      </c>
+      <c r="B1129" s="17" t="s">
+        <v>3081</v>
+      </c>
+      <c r="C1129" s="18" t="s">
+        <v>3082</v>
+      </c>
+    </row>
+    <row r="1130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1130" s="17" t="s">
+        <v>3083</v>
+      </c>
+      <c r="B1130" s="17" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C1130" s="18" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="1131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1131" s="17" t="s">
+        <v>3084</v>
+      </c>
+      <c r="B1131" s="17" t="s">
+        <v>1359</v>
+      </c>
+      <c r="C1131" s="18" t="s">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="1132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1132" s="17" t="s">
+        <v>3085</v>
+      </c>
+      <c r="B1132" s="17" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C1132" s="18" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="1133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1133" s="17" t="s">
+        <v>3086</v>
+      </c>
+      <c r="B1133" s="17" t="s">
+        <v>1363</v>
+      </c>
+      <c r="C1133" s="18" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="1134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1134" s="17" t="s">
+        <v>3087</v>
+      </c>
+      <c r="B1134" s="17" t="s">
+        <v>1365</v>
+      </c>
+      <c r="C1134" s="18" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="1135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1135" s="17" t="s">
+        <v>3088</v>
+      </c>
+      <c r="B1135" s="17" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C1135" s="18" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="1136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1136" s="17" t="s">
+        <v>3089</v>
+      </c>
+      <c r="B1136" s="17" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C1136" s="18" t="s">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="1137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1137" s="17" t="s">
+        <v>3013</v>
+      </c>
+      <c r="B1137" s="17" t="s">
+        <v>3014</v>
+      </c>
+      <c r="C1137" s="18" t="s">
+        <v>3015</v>
+      </c>
+    </row>
+    <row r="1138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1138" s="17" t="s">
+        <v>3090</v>
+      </c>
+      <c r="B1138" s="17" t="s">
+        <v>3091</v>
+      </c>
+      <c r="C1138" s="18" t="s">
+        <v>3092</v>
+      </c>
+    </row>
+    <row r="1139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1139" s="17" t="s">
+        <v>3093</v>
+      </c>
+      <c r="B1139" s="17" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C1139" s="18" t="s">
+        <v>1394</v>
+      </c>
+    </row>
+    <row r="1140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1140" s="17" t="s">
+        <v>3016</v>
+      </c>
+      <c r="B1140" s="17" t="s">
+        <v>3017</v>
+      </c>
+      <c r="C1140" s="18" t="s">
+        <v>3018</v>
+      </c>
+    </row>
+    <row r="1141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1141" s="17" t="s">
+        <v>3019</v>
+      </c>
+      <c r="B1141" s="17" t="s">
+        <v>3020</v>
+      </c>
+      <c r="C1141" s="18" t="s">
+        <v>3021</v>
+      </c>
+    </row>
+    <row r="1142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1142" s="17" t="s">
+        <v>3094</v>
+      </c>
+      <c r="B1142" s="17" t="s">
+        <v>1398</v>
+      </c>
+      <c r="C1142" s="18" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="1143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1143" s="17" t="s">
+        <v>3095</v>
+      </c>
+      <c r="B1143" s="17" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C1143" s="18" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="1144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1144" s="17" t="s">
+        <v>3096</v>
+      </c>
+      <c r="B1144" s="17" t="s">
+        <v>1406</v>
+      </c>
+      <c r="C1144" s="18" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="1145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1145" s="17" t="s">
+        <v>3097</v>
+      </c>
+      <c r="B1145" s="17" t="s">
+        <v>1408</v>
+      </c>
+      <c r="C1145" s="18" t="s">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="1146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1146" s="17" t="s">
+        <v>3098</v>
+      </c>
+      <c r="B1146" s="17" t="s">
+        <v>3099</v>
+      </c>
+      <c r="C1146" s="18" t="s">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="1147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1147" s="17" t="s">
+        <v>3101</v>
+      </c>
+      <c r="B1147" s="17" t="s">
+        <v>3102</v>
+      </c>
+      <c r="C1147" s="18" t="s">
+        <v>3103</v>
+      </c>
+    </row>
+    <row r="1148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1148" s="17" t="s">
+        <v>3104</v>
+      </c>
+      <c r="B1148" s="17" t="s">
+        <v>3105</v>
+      </c>
+      <c r="C1148" s="18" t="s">
+        <v>3106</v>
+      </c>
+    </row>
+    <row r="1149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1149" s="17" t="s">
+        <v>3022</v>
+      </c>
+      <c r="B1149" s="17" t="s">
+        <v>3023</v>
+      </c>
+      <c r="C1149" s="18" t="s">
+        <v>3024</v>
+      </c>
+    </row>
+    <row r="1150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1150" s="17" t="s">
+        <v>3025</v>
+      </c>
+      <c r="B1150" s="17" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C1150" s="18" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="1151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1151" s="17" t="s">
+        <v>3107</v>
+      </c>
+      <c r="B1151" s="17" t="s">
+        <v>1422</v>
+      </c>
+      <c r="C1151" s="18" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="1152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1152" s="17" t="s">
+        <v>3108</v>
+      </c>
+      <c r="B1152" s="17" t="s">
+        <v>3109</v>
+      </c>
+      <c r="C1152" s="18" t="s">
+        <v>3110</v>
+      </c>
+    </row>
+    <row r="1153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1153" s="17" t="s">
+        <v>3111</v>
+      </c>
+      <c r="B1153" s="17" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C1153" s="18" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="1154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1154" s="17" t="s">
+        <v>3112</v>
+      </c>
+      <c r="B1154" s="17" t="s">
+        <v>3113</v>
+      </c>
+      <c r="C1154" s="18" t="s">
+        <v>3114</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <conditionalFormatting sqref="B506 B815:B817">
@@ -29713,6 +30765,83 @@
     <hyperlink ref="C1075" r:id="rId1069" display="https://instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/slifmasina-uglovaa-metabo-w-13-150-quick"/>
     <hyperlink ref="C1076" r:id="rId1070" display="https://instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/slifmasina-uglovaa-metabo-wev-11-125-quick"/>
     <hyperlink ref="C1077" r:id="rId1071" display="https://instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/shlifmashina-uglovaya-metabo-wev-15-125-quick"/>
+    <hyperlink ref="C1078" r:id="rId1072" display="https://instrument.ms/raskhodnye-materialy-i-osnastka/osnastka-dlya-elektroinstrumenta/akkumulyatory-dlya-instrumenta/tm-metabo/akkumulator-3-st-zu-asc30-metabo-basic-set-52-lihd"/>
+    <hyperlink ref="C1079" r:id="rId1073" display="https://instrument.ms/raskhodnye-materialy-i-osnastka/osnastka-dlya-elektroinstrumenta/akkumulyatory-dlya-instrumenta/tm-metabo/akkumulator-li-power-metabo-18-v-20-ac"/>
+    <hyperlink ref="C1080" r:id="rId1074" display="https://instrument.ms/raskhodnye-materialy-i-osnastka/osnastka-dlya-elektroinstrumenta/akkumulyatory-dlya-instrumenta/tm-metabo/akkumulator-power-extreme-metabo-18-v-40-ac"/>
+    <hyperlink ref="C1081" r:id="rId1075" display="https://instrument.ms/elektroinstrument/lobziki-i-sabelnye-pily/sabelnye-pily-akkumulyatornye/tm-metabo/akkumulatornaa-sabelnaa-pila-metabo-sse-18-ltx-compact-2"/>
+    <hyperlink ref="C1082" r:id="rId1076" display="https://instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye-akkumulyatornye/tm-metabo/akkumulatornaa-uglovaa-slifmasina-metabo-w-18-ltx-125-2"/>
+    <hyperlink ref="C1083" r:id="rId1077" display="https://instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye-akkumulyatornye/tm-metabo/akkumulatornaa-uglovaa-slifmasina-metabo-wb-18-ltx-bl-125-quick"/>
+    <hyperlink ref="C1084" r:id="rId1078" display="https://instrument.ms/elektroinstrument/lobziki-i-sabelnye-pily/lobziki-akkumulyatornye/tm-metabo/akkumulatornyj-lobzik-metabo-stab-18-ltx-100-2"/>
+    <hyperlink ref="C1085" r:id="rId1079" display="https://instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-metabo/akkumulatornyj-surupovert-metabo-bs-144"/>
+    <hyperlink ref="C1086" r:id="rId1080" display="https://instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-metabo/akkumulatornyj-surupovert-metabo-bs-14415"/>
+    <hyperlink ref="C1087" r:id="rId1081" display="https://instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-metabo/akkumulyatornyi-shurupovert-metabo-bs-14-4-2-0"/>
+    <hyperlink ref="C1088" r:id="rId1082" display="https://instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-metabo/akkumulatornyj-surupovert-metabo-bs-18-l"/>
+    <hyperlink ref="C1089" r:id="rId1083" display="https://instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-metabo/akkumulatornyj-surupovert-metabo-bs-18-ltx-bl-i-3"/>
+    <hyperlink ref="C1090" r:id="rId1084" display="https://instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-metabo/akkumulatornyj-surupovert-metabo-bs-18-ltx-bl-i-4"/>
+    <hyperlink ref="C1091" r:id="rId1085" display="https://instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-metabo/akkumulatornyj-surupovert-metabo-bs-1815"/>
+    <hyperlink ref="C1092" r:id="rId1086" display="https://instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-metabo/akkumulatornyj-surupovert-metabo-bs-1820"/>
+    <hyperlink ref="C1093" r:id="rId1087" display="https://instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-metabo/akkumulatornyj-surupovert-metabo-bs18-ltx-bl-i"/>
+    <hyperlink ref="C1094" r:id="rId1088" display="https://instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-metabo/akkumulyatornyi-shurupovert-metabo-bs18-ltx-imp"/>
+    <hyperlink ref="C1095" r:id="rId1089" display="https://instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-metabo/akkumulatornyj-surupovert-metabo-powermaxx-bs-2"/>
+    <hyperlink ref="C1096" r:id="rId1090" display="https://instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-metabo/akkumulatornyj-surupovert-metabo-powermaxx-bs-4"/>
+    <hyperlink ref="C1097" r:id="rId1091" display="https://instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-metabo/akkumulatornyj-surupovert-metabo-powermaxx-bs-12"/>
+    <hyperlink ref="C1098" r:id="rId1092" display="https://instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-metabo/akkumulatornyj-surupovert-metabo-powermaxx-bs-12-bl"/>
+    <hyperlink ref="C1099" r:id="rId1093" display="https://instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-metabo/akkumulyatornyi-shurupovert-metabo-powermaxx-bs"/>
+    <hyperlink ref="C1100" r:id="rId1094" display="https://instrument.ms/elektroinstrument/dreli-i-miksery/dreli/tm-metabo/drel-udarnaya-metabo-sbe-650-1"/>
+    <hyperlink ref="C1101" r:id="rId1095" display="https://instrument.ms/elektroinstrument/dreli-i-miksery/dreli/tm-metabo/drel-udarnaya-metabo-sbe-650"/>
+    <hyperlink ref="C1102" r:id="rId1096" display="https://instrument.ms/raskhodnye-materialy-i-osnastka/osnastka-dlya-stankov/pilnye-polotna/tm-metabo/lenta-pilnaa-metabo-bas-260-1712h12h036"/>
+    <hyperlink ref="C1103" r:id="rId1097" display="https://instrument.ms/raskhodnye-materialy-i-osnastka/osnastka-dlya-stankov/pilnye-polotna/tm-metabo/lenta-pilnaa-metabo-bas-260-1712h6h036"/>
+    <hyperlink ref="C1104" r:id="rId1098" display="https://instrument.ms/elektroinstrument/lobziki-i-sabelnye-pily/lobziki/tm-metabo/lobzik-metabo-steb-140-plus"/>
+    <hyperlink ref="C1105" r:id="rId1099" display="https://instrument.ms/elektroinstrument/lobziki-i-sabelnye-pily/lobziki/tm-metabo/lobzik-metabo-steb-65-quick"/>
+    <hyperlink ref="C1106" r:id="rId1100" display="https://instrument.ms/elektroinstrument/lobziki-i-sabelnye-pily/lobziki/tm-metabo/lobzik-metabo-steb-70-quick"/>
+    <hyperlink ref="C1107" r:id="rId1101" display="https://instrument.ms/elektroinstrument/lobziki-i-sabelnye-pily/lobziki/tm-metabo/lobzik-metabo-steb-70-quick-1"/>
+    <hyperlink ref="C1108" r:id="rId1102" display="https://instrument.ms/pnevmaticheskoe-oborudovanie/pnevmoinstrument/pnevmoshlifovalnye-mashiny-pryamye/tm-metabo/masina-slifovalnaa-pramaa-metabo-dg-25-set"/>
+    <hyperlink ref="C1109" r:id="rId1103" display="https://instrument.ms/raskhodnye-materialy-i-osnastka/osnastka-dlya-elektroinstrumenta/bity/tm-metabo/nabor-bit-metabo-32-sht"/>
+    <hyperlink ref="C1110" r:id="rId1104" display="https://instrument.ms/raskhodnye-materialy-i-osnastka/osnastka-dlya-elektroinstrumenta/bity/tm-metabo/nabor-bit-metabo-8sht-universalnyi-derzhatel"/>
+    <hyperlink ref="C1111" r:id="rId1105" display="https://instrument.ms/raskhodnye-materialy-i-osnastka/osnastka-dlya-elektroinstrumenta/sverla/tm-metabo/nabor-sverl-po-metallu-hss-g-metabo-d-1-13-mm-25-sht"/>
+    <hyperlink ref="C1112" r:id="rId1106" display="https://instrument.ms/raskhodnye-materialy-i-osnastka/osnastka-dlya-elektroinstrumenta/sverla/tm-metabo/nabor-sverl-po-metallu-hss-r-metabo-d-1-10-mm-19-sht"/>
+    <hyperlink ref="C1113" r:id="rId1107" display="https://instrument.ms/raskhodnye-materialy-i-osnastka/osnastka-dlya-elektroinstrumenta/sverla/tm-metabo/nabor-sverl-po-metallu-hss-r-metabo-d-1-13-mm-25-sht"/>
+    <hyperlink ref="C1114" r:id="rId1108" display="https://instrument.ms/raskhodnye-materialy-i-osnastka/osnastka-dlya-elektroinstrumenta/sverla/tm-metabo/nabor-sverl-po-metallu-hss-tin-metabo-d-1-10-mm-19-sht"/>
+    <hyperlink ref="C1115" r:id="rId1109" display="https://instrument.ms/sistemy-vodosnabzheniya/nasosnye-stantsii/tm-metabo/nasosnaya-stantsiya-metabo-hww-4500-25-inox"/>
+    <hyperlink ref="C1116" r:id="rId1110" display="https://instrument.ms/raskhodnye-materialy-i-osnastka/osnastka-dlya-stankov/nozhi-k-stankam/tm-metabo/nozhi-k-reismusu-metavo-dh330-metabo-hss-332"/>
+    <hyperlink ref="C1117" r:id="rId1111" display="https://instrument.ms/raskhodnye-materialy-i-osnastka/osnastka-dlya-elektroinstrumenta/krugi-otreznye/tm-metabo/otreznoi-krug-po-metallu-metabo-125kh2-5kh22-sp-novoflex"/>
+    <hyperlink ref="C1118" r:id="rId1112" display="https://instrument.ms/raskhodnye-materialy-i-osnastka/osnastka-dlya-elektroinstrumenta/krugi-otreznye/tm-metabo/otreznoj-krug-po-metallu-nerzavejke-metabo-125h10h22-sp-novorapid"/>
+    <hyperlink ref="C1119" r:id="rId1113" display="https://instrument.ms/raskhodnye-materialy-i-osnastka/osnastka-dlya-elektroinstrumenta/krugi-otreznye/tm-metabo/otreznoj-krug-po-metallu-nerzavejke-metabo-230h19h22-sp-novorapid"/>
+    <hyperlink ref="C1120" r:id="rId1114" display="https://instrument.ms/raskhodnye-materialy-i-osnastka/osnastka-dlya-elektroinstrumenta/krugi-otreznye/tm-metabo/otreznoj-krug-po-metallu-nerzavejke-metabo-230h25h22-sp-novorapid"/>
+    <hyperlink ref="C1121" r:id="rId1115" display="https://instrument.ms/elektroinstrument/perforatory/perforatory-sds-max/tm-metabo/perforator-sds-max-metabo-knev-5-40-bl"/>
+    <hyperlink ref="C1122" r:id="rId1116" display="https://instrument.ms/elektroinstrument/perforatory/perforatory-sds-setevye/tm-metabo/perforator-sds-metabo-khe-2444-2"/>
+    <hyperlink ref="C1123" r:id="rId1117" display="https://instrument.ms/elektroinstrument/perforatory/perforatory-sds-setevye/tm-metabo/perforator-sds-metabo-khe-2644-2"/>
+    <hyperlink ref="C1124" r:id="rId1118" display="https://instrument.ms/elektroinstrument/perforatory/perforatory-sds-setevye/tm-metabo/perforator-sds-metabo-khe-2660-quick-2"/>
+    <hyperlink ref="C1125" r:id="rId1119" display="https://instrument.ms/elektroinstrument/perforatory/perforatory-sds-setevye/tm-metabo/perforator-sds-metabo-khe-2660-quick"/>
+    <hyperlink ref="C1126" r:id="rId1120" display="https://instrument.ms/elektroinstrument/perforatory/perforatory-sds-setevye/tm-metabo/perforator-sds-metabo-khe-2860-quick"/>
+    <hyperlink ref="C1127" r:id="rId1121" display="https://instrument.ms/elektroinstrument/perforatory/perforatory-sds-akkumulyatornye/tm-metabo/perforator-akkumulatornyj-metabo-kha-18-ltx-2"/>
+    <hyperlink ref="C1128" r:id="rId1122" display="https://instrument.ms/elektroinstrument/pily-diskovye/pily-diskovye-setevye/tm-metabo/pila-diskovaya-metabo-ks-55"/>
+    <hyperlink ref="C1129" r:id="rId1123" display="https://instrument.ms/elektroinstrument/pily-diskovye/pily-diskovye-setevye/tm-metabo/pila-diskovaa-metabo-ks-66-fs"/>
+    <hyperlink ref="C1130" r:id="rId1124" display="https://instrument.ms/elektroinstrument/pily-diskovye/pily-diskovye-akkumulyatornye/tm-metabo/pila-diskovaa-akkumulatornaa-metabo-ks-18-ltx-57"/>
+    <hyperlink ref="C1131" r:id="rId1125" display="https://instrument.ms/stanki/pily-tortsovochnye/tm-metabo/pila-tortsovochnaya-metabo-kgs-216-m-lasercut"/>
+    <hyperlink ref="C1132" r:id="rId1126" display="https://instrument.ms/stanki/pily-tortsovochnye/tm-metabo/pila-tortsovochnaya-metabo-kgs-254-m"/>
+    <hyperlink ref="C1133" r:id="rId1127" display="https://instrument.ms/stanki/pily-tortsovochnye/tm-metabo/pila-tortsovochnaya-metabo-kgs-305-m"/>
+    <hyperlink ref="C1134" r:id="rId1128" display="https://instrument.ms/stanki/pily-tortsovochnye/tm-metabo/pila-tortsovochnaya-metabo-ks-216-m-lasercut"/>
+    <hyperlink ref="C1135" r:id="rId1129" display="https://instrument.ms/elektroinstrument/feny-stroitelnye-i-payalnye-pistolety/feny-stroitelnye/tm-metabo/pistolet-goryachego-vozdukha-metabo-h-16-500"/>
+    <hyperlink ref="C1136" r:id="rId1130" display="https://instrument.ms/stanki/stanki-reismusovye-i-strogalnye/tm-metabo/stanok-derevoobrabatyvayushchii-reismusovyi-metabo-dn-330"/>
+    <hyperlink ref="C1137" r:id="rId1131" display="https://instrument.ms/raskhodnye-materialy-i-osnastka/osnastka-dlya-elektroinstrumenta/komplektuyushchie-i-zapchasti-dlya-elektroinstrumenta/tm-metabo/sumka-dla-instrumenta-metabo-bolsaa"/>
+    <hyperlink ref="C1138" r:id="rId1132" display="https://instrument.ms/raskhodnye-materialy-i-osnastka/osnastka-dlya-elektroinstrumenta/komplektuyushchie-i-zapchasti-dlya-elektroinstrumenta/tm-metabo/sumka-dla-instrumenta-metabo-malaa"/>
+    <hyperlink ref="C1139" r:id="rId1133" display="https://instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/slifmasina-uglovaa-metabo-w-1100-125"/>
+    <hyperlink ref="C1140" r:id="rId1134" display="https://instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/slifmasina-uglovaa-metabo-w-13-125-quick"/>
+    <hyperlink ref="C1141" r:id="rId1135" display="https://instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/slifmasina-uglovaa-metabo-w-13-150-quick"/>
+    <hyperlink ref="C1142" r:id="rId1136" display="https://instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/slifmasina-uglovaa-metabo-w-2200-230-2"/>
+    <hyperlink ref="C1143" r:id="rId1137" display="https://instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/slifmasina-uglovaa-metabo-w-850-125"/>
+    <hyperlink ref="C1144" r:id="rId1138" display="https://instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/slifmasina-uglovaa-metabo-we-1500-150-rt"/>
+    <hyperlink ref="C1145" r:id="rId1139" display="https://instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/shlifmashina-uglovaya-metabo-we-15-125-quick"/>
+    <hyperlink ref="C1146" r:id="rId1140" display="https://instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/slifmasina-uglovaa-metabo-we-2000-230"/>
+    <hyperlink ref="C1147" r:id="rId1141" display="https://instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/slifmasina-uglovaa-metabo-we-2200-230"/>
+    <hyperlink ref="C1148" r:id="rId1142" display="https://instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/slifmasina-uglovaa-metabo-we-24-230-mvt"/>
+    <hyperlink ref="C1149" r:id="rId1143" display="https://instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/slifmasina-uglovaa-metabo-wev-11-125-quick"/>
+    <hyperlink ref="C1150" r:id="rId1144" display="https://instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/shlifmashina-uglovaya-metabo-wev-15-125-quick"/>
+    <hyperlink ref="C1151" r:id="rId1145" display="https://instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/slifmasina-uglovaa-metabo-wev-850-125"/>
+    <hyperlink ref="C1152" r:id="rId1146" display="https://instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-metabo/slifmasina-uglovaa-metabo-wq-1100-125-quick"/>
+    <hyperlink ref="C1153" r:id="rId1147" display="https://instrument.ms/elektroinstrument/shlifovalnye-mashiny/shlifmashiny-ekstsentrikovye/tm-metabo/slifmasina-ekscentrikovaa-metabo-fsx-200-intec"/>
+    <hyperlink ref="C1154" r:id="rId1148" display="https://instrument.ms/elektroinstrument/shlifovalnye-mashiny/shlifmashiny-ekstsentrikovye/tm-metabo/slifmasina-ekscentrikovaa-metabo-sxe-3125"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
add new item for parsing
</commit_message>
<xml_diff>
--- a/data/Instrument_prices.xlsx
+++ b/data/Instrument_prices.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3302" uniqueCount="3119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3304" uniqueCount="3121">
   <si>
     <t xml:space="preserve">наш код</t>
   </si>
@@ -9377,6 +9377,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://instrument.ms/elektroinstrument/pily-diskovye/pily-diskovye-akkumulyatornye/tm-metabo/pila-diskovaa-akkumulatornaa-metabo-ks-18-ltx-57-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Пила дисковая Bosch HD GKS 140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://kirov.instrument.ms/elektroinstrument/pily-diskovye/pily-diskovye-setevye/tm-bosch/pila-diskovaa-bosch-hd-gks-140</t>
   </si>
 </sst>
 </file>
@@ -9703,7 +9709,7 @@
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1139" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1159" activeCellId="0" sqref="B1159"/>
+      <selection pane="topLeft" activeCell="B1162" activeCellId="0" sqref="B1162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29673,6 +29679,17 @@
       </c>
       <c r="C1157" s="18" t="s">
         <v>3118</v>
+      </c>
+    </row>
+    <row r="1158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1158" s="0" t="n">
+        <v>106288</v>
+      </c>
+      <c r="B1158" s="0" t="s">
+        <v>3119</v>
+      </c>
+      <c r="C1158" s="18" t="s">
+        <v>3120</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
add new row for compare
</commit_message>
<xml_diff>
--- a/data/Instrument_prices.xlsx
+++ b/data/Instrument_prices.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3304" uniqueCount="3121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3306" uniqueCount="3123">
   <si>
     <t xml:space="preserve">наш код</t>
   </si>
@@ -9383,6 +9383,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://kirov.instrument.ms/elektroinstrument/pily-diskovye/pily-diskovye-setevye/tm-bosch/pila-diskovaa-bosch-hd-gks-140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Аккумуляторная угловая шлифмашина Bosch HD GWS 180-Li</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye-akkumulyatornye/tm-bosch/akkumulatornaa-uglovaa-slifmasina-bosch-hd-gws-180-li</t>
   </si>
 </sst>
 </file>
@@ -9709,7 +9715,7 @@
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1139" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1162" activeCellId="0" sqref="B1162"/>
+      <selection pane="topLeft" activeCell="B1156" activeCellId="0" sqref="B1156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29690,6 +29696,17 @@
       </c>
       <c r="C1158" s="18" t="s">
         <v>3120</v>
+      </c>
+    </row>
+    <row r="1159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1159" s="0" t="n">
+        <v>99118</v>
+      </c>
+      <c r="B1159" s="0" t="s">
+        <v>3121</v>
+      </c>
+      <c r="C1159" s="18" t="s">
+        <v>3122</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
add more rows for compare
</commit_message>
<xml_diff>
--- a/data/Instrument_prices.xlsx
+++ b/data/Instrument_prices.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3306" uniqueCount="3123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3310" uniqueCount="3126">
   <si>
     <t xml:space="preserve">наш код</t>
   </si>
@@ -9389,6 +9389,15 @@
   </si>
   <si>
     <t xml:space="preserve">https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye-akkumulyatornye/tm-bosch/akkumulatornaa-uglovaa-slifmasina-bosch-hd-gws-180-li</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://kirov.instrument.ms/elektroinstrument/lobziki-i-sabelnye-pily/sabelnye-pily-setevye/tm-bosch/elektropila-sabelnaya-bosch-gsa-1300-pce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Шлифмашина угловая Bosch HD GWS 2200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://kirov.instrument.ms/elektroinstrument/ushm-bolgarki/shlifmashiny-uglovye/tm-bosch/slifmasina-uglovaa-bosch-gws-580</t>
   </si>
 </sst>
 </file>
@@ -9715,7 +9724,7 @@
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1139" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1156" activeCellId="0" sqref="B1156"/>
+      <selection pane="topLeft" activeCell="B1161" activeCellId="0" sqref="B1161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29707,6 +29716,28 @@
       </c>
       <c r="C1159" s="18" t="s">
         <v>3122</v>
+      </c>
+    </row>
+    <row r="1160" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1160" s="0" t="n">
+        <v>28675</v>
+      </c>
+      <c r="B1160" s="5" t="s">
+        <v>737</v>
+      </c>
+      <c r="C1160" s="18" t="s">
+        <v>3123</v>
+      </c>
+    </row>
+    <row r="1161" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1161" s="0" t="n">
+        <v>98022</v>
+      </c>
+      <c r="B1161" s="5" t="s">
+        <v>3124</v>
+      </c>
+      <c r="C1161" s="18" t="s">
+        <v>3125</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
add 4 new rows
</commit_message>
<xml_diff>
--- a/data/Instrument_prices.xlsx
+++ b/data/Instrument_prices.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3314" uniqueCount="3129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3322" uniqueCount="3137">
   <si>
     <t xml:space="preserve">наш код</t>
   </si>
@@ -9407,6 +9407,30 @@
   </si>
   <si>
     <t xml:space="preserve">https://kirov.instrument.ms/elektroinstrument/shlifovalnye-mashiny/shlifmashiny-ekstsentrikovye/tm-bosch/shlifmashina-ekstsentrikovaya-bosch-gex-125-1-ae-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Аккумуляторный шуруповерт Metabo BS 18 LT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://kirov.instrument.ms/elektroinstrument/shurupoverty-i-otvertki/shurupoverty-akkumulyatornye/tm-metabo/akkumulatornyj-surupovert-metabo-bs-18-lt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Пистолет горячего воздуха Metabo HG 16-500 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://kirov.instrument.ms/elektroinstrument/feny-stroitelnye-i-payalnye-pistolety/feny-stroitelnye/tm-metabo/pistolet-goracego-vozduha-metabo-hg-16-500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дрель ударная Metabo SBE 650 600671000/600742000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://kirov.instrument.ms/elektroinstrument/dreli-i-miksery/dreli/tm-metabo/drel-udarnaya-metabo-sbe-650-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дрель ударная Metabo SBE 650 600671850/600742850</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://kirov.instrument.ms/elektroinstrument/dreli-i-miksery/dreli/tm-metabo/drel-udarnaya-metabo-sbe-650</t>
   </si>
 </sst>
 </file>
@@ -9733,7 +9757,7 @@
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1139" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1163" activeCellId="0" sqref="A1163"/>
+      <selection pane="topLeft" activeCell="B1167" activeCellId="0" sqref="B1167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29769,6 +29793,50 @@
       </c>
       <c r="C1163" s="18" t="s">
         <v>3128</v>
+      </c>
+    </row>
+    <row r="1164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1164" s="0" t="n">
+        <v>104831</v>
+      </c>
+      <c r="B1164" s="0" t="s">
+        <v>3129</v>
+      </c>
+      <c r="C1164" s="0" t="s">
+        <v>3130</v>
+      </c>
+    </row>
+    <row r="1165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1165" s="0" t="n">
+        <v>102651</v>
+      </c>
+      <c r="B1165" s="0" t="s">
+        <v>3131</v>
+      </c>
+      <c r="C1165" s="0" t="s">
+        <v>3132</v>
+      </c>
+    </row>
+    <row r="1166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1166" s="0" t="n">
+        <v>104158</v>
+      </c>
+      <c r="B1166" s="0" t="s">
+        <v>3133</v>
+      </c>
+      <c r="C1166" s="0" t="s">
+        <v>3134</v>
+      </c>
+    </row>
+    <row r="1167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1167" s="0" t="n">
+        <v>105352</v>
+      </c>
+      <c r="B1167" s="0" t="s">
+        <v>3135</v>
+      </c>
+      <c r="C1167" s="0" t="s">
+        <v>3136</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
add one more string to parsing-list
</commit_message>
<xml_diff>
--- a/data/Instrument_prices.xlsx
+++ b/data/Instrument_prices.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3322" uniqueCount="3137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3324" uniqueCount="3139">
   <si>
     <t xml:space="preserve">наш код</t>
   </si>
@@ -9431,6 +9431,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://kirov.instrument.ms/elektroinstrument/dreli-i-miksery/dreli/tm-metabo/drel-udarnaya-metabo-sbe-650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Пила торцовочная Bosch GCM 216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://kirov.instrument.ms/stanki/pily-tortsovochnye/tm-bosch/pila-torcovocnaa-bosch-gcm-216</t>
   </si>
 </sst>
 </file>
@@ -9757,7 +9763,7 @@
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1139" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1167" activeCellId="0" sqref="B1167"/>
+      <selection pane="topLeft" activeCell="B1166" activeCellId="0" sqref="B1166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29837,6 +29843,17 @@
       </c>
       <c r="C1167" s="0" t="s">
         <v>3136</v>
+      </c>
+    </row>
+    <row r="1168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1168" s="0" t="n">
+        <v>106628</v>
+      </c>
+      <c r="B1168" s="0" t="s">
+        <v>3137</v>
+      </c>
+      <c r="C1168" s="0" t="s">
+        <v>3138</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>